<commit_message>
Deploying to gh-pages from  @ 47d14905be37ec9798fbb55fa210b3ddab1220dd 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-2-5.xlsx
+++ b/assets/excel/2021_1-2-5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BBA53C-192B-4E7A-B271-FC6970F2BC97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35AC7140-1EE3-47C0-9BD1-CDB54936F581}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{6FA2B562-512B-4618-9F66-F48F7F0E5473}"/>
   </bookViews>
@@ -475,8 +475,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -484,15 +498,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -507,11 +512,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -831,8 +833,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:I279"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A262" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,52 +874,52 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
@@ -6165,7 +6167,7 @@
       <c r="G273" s="9"/>
     </row>
     <row r="274" spans="2:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B274" s="16" t="s">
+      <c r="B274" s="29" t="s">
         <v>50</v>
       </c>
       <c r="E274" s="9"/>
@@ -6191,7 +6193,7 @@
       </c>
     </row>
     <row r="279" spans="2:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B279" s="17" t="s">
+      <c r="B279" s="16" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ fb3091c2372595beb9b1f1785ea0c8c72c6980e7 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-2-5.xlsx
+++ b/assets/excel/2021_1-2-5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35AC7140-1EE3-47C0-9BD1-CDB54936F581}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A87851-1260-4072-8DE3-DDD8D105C612}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{6FA2B562-512B-4618-9F66-F48F7F0E5473}"/>
   </bookViews>
@@ -476,6 +476,9 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -511,9 +514,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -833,8 +833,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:I279"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,52 +874,52 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="18"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="2:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="19"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="24"/>
-      <c r="C10" s="19"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
@@ -1269,7 +1269,7 @@
         <v>2020</v>
       </c>
       <c r="D28" s="11">
-        <v>368165</v>
+        <v>351275</v>
       </c>
       <c r="E28" s="12">
         <v>55.560686105414689</v>
@@ -6167,7 +6167,7 @@
       <c r="G273" s="9"/>
     </row>
     <row r="274" spans="2:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B274" s="29" t="s">
+      <c r="B274" s="17" t="s">
         <v>50</v>
       </c>
       <c r="E274" s="9"/>

</xml_diff>